<commit_message>
Update eye blink function
</commit_message>
<xml_diff>
--- a/Data_visualization/eye_blink_detection_results.xlsx
+++ b/Data_visualization/eye_blink_detection_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,194 +436,203 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Start Time</t>
+          <t>Gesture</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>End Time</t>
+          <t>Ground_Truth</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Ground Truth</t>
+          <t>Detected_Blink</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Detected Eye Blink</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Both_Eyeblink</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Both_EyeBlink_Left_Head_Move.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>19</v>
-      </c>
-      <c r="B2" t="n">
-        <v>21</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>23</v>
-      </c>
-      <c r="B3" t="n">
-        <v>26</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Both_EyeBlink_Right_Head_Move.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Left_EyeBlink_Right_Head_Move.jpg</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>28</v>
-      </c>
-      <c r="B4" t="n">
-        <v>31</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>No Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Right_EyeBlink_Left_Head_Move</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Both_Eyeblink</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Both_EyeBlink_Left_Head_Move.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Both_EyeBlink_Right_Head_Move.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Left_EyeBlink_Right_Head_Move.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>34</v>
-      </c>
-      <c r="B5" t="n">
-        <v>37</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>39</v>
-      </c>
-      <c r="B6" t="n">
-        <v>42</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Right_EyeBlink_Left_Head_Move</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>2</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>43</v>
-      </c>
-      <c r="B7" t="n">
-        <v>45</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>48</v>
-      </c>
-      <c r="B8" t="n">
-        <v>52</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>55</v>
-      </c>
-      <c r="B9" t="n">
-        <v>58</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>61</v>
-      </c>
-      <c r="B10" t="n">
-        <v>64</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>67</v>
-      </c>
-      <c r="B11" t="n">
-        <v>70</v>
-      </c>
       <c r="C11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>No Match</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add eye blink v2 func
</commit_message>
<xml_diff>
--- a/Data_visualization/eye_blink_detection_results.xlsx
+++ b/Data_visualization/eye_blink_detection_results.xlsx
@@ -464,12 +464,10 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>No Blink Detected</t>
         </is>
       </c>
     </row>
@@ -519,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -537,11 +535,11 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -554,12 +552,10 @@
       <c r="B7" t="n">
         <v>0</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Match</t>
+          <t>No Blink Detected</t>
         </is>
       </c>
     </row>
@@ -591,11 +587,11 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Match</t>
+          <t>No Match</t>
         </is>
       </c>
     </row>
@@ -609,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -627,11 +623,11 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Match</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimize parameters, Data upload
</commit_message>
<xml_diff>
--- a/Data_visualization/eye_blink_detection_results.xlsx
+++ b/Data_visualization/eye_blink_detection_results.xlsx
@@ -465,11 +465,11 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Match</t>
+          <t>No Match</t>
         </is>
       </c>
     </row>
@@ -500,42 +500,44 @@
       <c r="B4" t="n">
         <v>0</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>No Blink Detected</t>
+          <t>Match</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Both_EyeBlink_Left_Head_Move</t>
+          <t>Left_EyeBlink</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Match</t>
+          <t>No Match</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Both_EyeBlink_Right_Head_Move</t>
+          <t>Left_Head_Movement</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -546,36 +548,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Left_EyeBlink_Right_Head_Move</t>
+          <t>Right_EyeBlink</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Match</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Right_EyeBlink_Left_Head_Move</t>
+          <t>Right_Head_Movement</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Match</t>
+          <t>No Match</t>
         </is>
       </c>
     </row>
@@ -588,24 +590,26 @@
       <c r="B9" t="n">
         <v>0</v>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>No Blink Detected</t>
+          <t>Match</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Both_EyeBlink_Left_Head_Move</t>
+          <t>Left_EyeBlink</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -616,14 +620,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Both_EyeBlink_Right_Head_Move</t>
+          <t>Left_Head_Movement</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -634,36 +638,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Left_EyeBlink_Right_Head_Move</t>
+          <t>Right_EyeBlink</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>No Match</t>
+          <t>Match</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Right_EyeBlink_Left_Head_Move</t>
+          <t>Right_Head_Movement</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Match</t>
+          <t>No Match</t>
         </is>
       </c>
     </row>

</xml_diff>